<commit_message>
Update README.md and benchmark results
</commit_message>
<xml_diff>
--- a/sample/benchmarks/01_gear/data_sheet.xlsx
+++ b/sample/benchmarks/01_gear/data_sheet.xlsx
@@ -503,13 +503,13 @@
                 <c:formatCode>0.0_ </c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>4.0999999999999996</c:v>
+                  <c:v>5.8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>13.8</c:v>
+                  <c:v>22.3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>41.8</c:v>
+                  <c:v>198</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -579,11 +579,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="203643136"/>
-        <c:axId val="36466688"/>
+        <c:axId val="217401984"/>
+        <c:axId val="217411968"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="203643136"/>
+        <c:axId val="217401984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -593,7 +593,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="36466688"/>
+        <c:crossAx val="217411968"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -601,7 +601,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="36466688"/>
+        <c:axId val="217411968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -612,7 +612,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="203643136"/>
+        <c:crossAx val="217401984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1189,7 +1189,7 @@
   <dimension ref="B1:L30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1322,26 +1322,26 @@
         <v>10</v>
       </c>
       <c r="E5">
-        <v>6.1</v>
+        <v>6.9</v>
       </c>
       <c r="F5" s="7">
-        <v>4.0999999999999996</v>
+        <v>5.8</v>
       </c>
       <c r="G5" s="7">
-        <v>12.4</v>
+        <v>14.3</v>
       </c>
       <c r="H5" s="7">
         <f t="shared" si="0"/>
-        <v>8.3000000000000007</v>
+        <v>8.5</v>
       </c>
       <c r="I5" s="10">
         <v>334.16</v>
       </c>
       <c r="J5" s="6">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="K5" s="5">
-        <v>6.9213159999999997E-7</v>
+        <v>6.6381849999999998E-7</v>
       </c>
       <c r="L5" s="4">
         <v>9.9999999999999995E-7</v>
@@ -1460,26 +1460,26 @@
         <v>10</v>
       </c>
       <c r="E9" s="11">
-        <v>25.8</v>
+        <v>26.7</v>
       </c>
       <c r="F9" s="7">
-        <v>13.8</v>
+        <v>22.3</v>
       </c>
       <c r="G9" s="7">
-        <v>32.799999999999997</v>
+        <v>40.5</v>
       </c>
       <c r="H9" s="7">
         <f t="shared" si="0"/>
-        <v>18.999999999999996</v>
-      </c>
-      <c r="I9" s="10">
+        <v>18.2</v>
+      </c>
+      <c r="I9" s="2">
         <v>397.37</v>
       </c>
       <c r="J9" s="6">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="K9" s="5">
-        <v>9.7878530000000009E-7</v>
+        <v>6.8805879999999997E-7</v>
       </c>
       <c r="L9" s="4">
         <v>9.9999999999999995E-7</v>
@@ -1597,26 +1597,26 @@
         <v>10</v>
       </c>
       <c r="E13" s="11">
-        <v>72.400000000000006</v>
+        <v>79.400000000000006</v>
       </c>
       <c r="F13" s="7">
-        <v>41.8</v>
+        <v>198</v>
       </c>
       <c r="G13" s="7">
-        <v>93.2</v>
+        <v>256.3</v>
       </c>
       <c r="H13" s="7">
         <f>G13-F13</f>
-        <v>51.400000000000006</v>
+        <v>58.300000000000011</v>
       </c>
       <c r="I13" s="10">
         <v>442.02</v>
       </c>
       <c r="J13" s="6">
-        <v>29</v>
-      </c>
-      <c r="K13" s="4">
-        <v>7.756884E-7</v>
+        <v>12</v>
+      </c>
+      <c r="K13" s="5">
+        <v>3.0565990000000001E-7</v>
       </c>
       <c r="L13" s="4">
         <v>9.9999999999999995E-7</v>
@@ -1728,13 +1728,13 @@
         <v>10</v>
       </c>
       <c r="F22" s="7">
-        <v>4.0999999999999996</v>
+        <v>5.8</v>
       </c>
       <c r="G22" s="7">
-        <v>13.8</v>
+        <v>22.3</v>
       </c>
       <c r="H22" s="7">
-        <v>41.8</v>
+        <v>198</v>
       </c>
     </row>
     <row r="23" spans="3:8" x14ac:dyDescent="0.15">
@@ -1825,15 +1825,15 @@
       </c>
       <c r="F29" s="7">
         <f t="shared" si="3"/>
-        <v>18.5</v>
+        <v>21.200000000000003</v>
       </c>
       <c r="G29" s="7">
         <f t="shared" si="4"/>
-        <v>58.599999999999994</v>
+        <v>67.2</v>
       </c>
       <c r="H29" s="12">
         <f t="shared" si="5"/>
-        <v>165.60000000000002</v>
+        <v>335.70000000000005</v>
       </c>
     </row>
     <row r="30" spans="3:8" x14ac:dyDescent="0.15">

</xml_diff>